<commit_message>
Update: riccota models + fillers
</commit_message>
<xml_diff>
--- a/app/data/static/params/ricotta_old.xlsx
+++ b/app/data/static/params/ricotta_old.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,90 +451,95 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Вначале</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Название форм фактора</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Линия</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Имя бренда</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Вес нетто</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Коробки</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Вес форм фактора</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Выход</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Количество баков</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Скорость упаковки</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Подготовка полуфабриката</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Анализ</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Перекачка</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Нагрев</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Выдержка</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Сбор белка</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Заборс</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Слив</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Kод</t>
         </is>
@@ -555,7 +560,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -565,52 +570,57 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Unagrande</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.25</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>6</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>300</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>40</v>
       </c>
-      <c r="N2" t="n">
-        <v>10</v>
-      </c>
       <c r="O2" t="n">
         <v>10</v>
       </c>
       <c r="P2" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="n">
         <v>20</v>
       </c>
-      <c r="Q2" t="n">
-        <v>15</v>
-      </c>
       <c r="R2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U2" t="n">
         <v>5</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" t="inlineStr">
         <is>
           <t>Н0000094030</t>
         </is>
@@ -631,7 +641,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -641,52 +651,57 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Unagrande</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.5</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>6</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>300</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>2</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>25</v>
       </c>
-      <c r="N3" t="n">
-        <v>10</v>
-      </c>
       <c r="O3" t="n">
         <v>10</v>
       </c>
       <c r="P3" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q3" t="n">
         <v>20</v>
       </c>
-      <c r="Q3" t="n">
-        <v>15</v>
-      </c>
       <c r="R3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U3" t="n">
         <v>5</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V3" t="n">
+        <v>5</v>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>Н0000094029</t>
         </is>
@@ -707,7 +722,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -717,52 +732,57 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Aventino</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.2</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>6</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="n">
-        <v>400</v>
-      </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>600</v>
       </c>
       <c r="M4" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N4" t="n">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="O4" t="n">
         <v>10</v>
       </c>
       <c r="P4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="n">
         <v>20</v>
       </c>
-      <c r="Q4" t="n">
-        <v>15</v>
-      </c>
       <c r="R4" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U4" t="n">
         <v>5</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="V4" t="n">
+        <v>5</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>Н0000096235</t>
         </is>
@@ -783,7 +803,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -793,52 +813,57 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>Pretto</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.5</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>6</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="n">
-        <v>400</v>
-      </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>600</v>
       </c>
       <c r="M5" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="N5" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="O5" t="n">
         <v>10</v>
       </c>
       <c r="P5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="n">
         <v>20</v>
       </c>
-      <c r="Q5" t="n">
-        <v>15</v>
-      </c>
       <c r="R5" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U5" t="n">
         <v>5</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>Н0000086888</t>
         </is>
@@ -859,7 +884,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -869,52 +894,57 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Pretto</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>0.2</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>6</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="n">
-        <v>400</v>
-      </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>600</v>
       </c>
       <c r="M6" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N6" t="n">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="O6" t="n">
         <v>10</v>
       </c>
       <c r="P6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="n">
         <v>20</v>
       </c>
-      <c r="Q6" t="n">
-        <v>15</v>
-      </c>
       <c r="R6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U6" t="n">
         <v>5</v>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="V6" t="n">
+        <v>5</v>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>Н0000088471</t>
         </is>
@@ -935,7 +965,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -945,52 +975,57 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Фермерская коллекция</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.2</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>6</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="n">
-        <v>400</v>
-      </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>600</v>
       </c>
       <c r="M7" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N7" t="n">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="O7" t="n">
         <v>10</v>
       </c>
       <c r="P7" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q7" t="n">
         <v>20</v>
       </c>
-      <c r="Q7" t="n">
-        <v>15</v>
-      </c>
       <c r="R7" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T7" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U7" t="n">
         <v>5</v>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="V7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W7" t="inlineStr">
         <is>
           <t>Н0000095392</t>
         </is>
@@ -1002,16 +1037,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Рикотта "ВкусВилл", 45%, 0,18 кг, пл/с (6 шт)</t>
+          <t>Рикотта с ванилью "Красная птица", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>45</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Ваниль</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1021,54 +1060,59 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ВкусВилл</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>0.18</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Красная птица</t>
+        </is>
       </c>
       <c r="I8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J8" t="n">
         <v>6</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0</v>
       </c>
-      <c r="K8" t="n">
-        <v>400</v>
-      </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="M8" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="N8" t="n">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="O8" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P8" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q8" t="n">
         <v>20</v>
       </c>
-      <c r="Q8" t="n">
-        <v>15</v>
-      </c>
       <c r="R8" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S8" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U8" t="n">
-        <v>5</v>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>Н0000093950</t>
+        <v>15</v>
+      </c>
+      <c r="V8" t="n">
+        <v>5</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Н0000096627</t>
         </is>
       </c>
     </row>
@@ -1078,16 +1122,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Рикотта "Красная птица", 30%,  0,25 кг, пл/с (6 шт)</t>
+          <t>Рикотта шоколадно-ореховая "Красная птица", 35%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Шоколад-орех</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1097,54 +1145,59 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>Красная птица</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>0.25</v>
-      </c>
       <c r="I9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J9" t="n">
         <v>6</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="n">
-        <v>200</v>
-      </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>350</v>
       </c>
       <c r="M9" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="N9" t="n">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="O9" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="P9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q9" t="n">
         <v>20</v>
       </c>
-      <c r="Q9" t="n">
-        <v>15</v>
-      </c>
       <c r="R9" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U9" t="n">
-        <v>5</v>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>Н0000095119</t>
+        <v>15</v>
+      </c>
+      <c r="V9" t="n">
+        <v>5</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Н0000096629</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1207,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Рикотта с ванилью "Красная птица", 30%, 0,2 кг, пл/с</t>
+          <t>Рикотта с ванилью "Бонджорно", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1167,7 +1220,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1177,54 +1230,59 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Красная птица</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Бонджорно</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
         <v>0.2</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>6</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>250</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>2</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>28</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>30</v>
       </c>
-      <c r="O10" t="n">
-        <v>10</v>
-      </c>
       <c r="P10" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q10" t="n">
         <v>20</v>
       </c>
-      <c r="Q10" t="n">
-        <v>15</v>
-      </c>
       <c r="R10" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T10" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U10" t="n">
-        <v>5</v>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>Н0000096627</t>
+        <v>15</v>
+      </c>
+      <c r="V10" t="n">
+        <v>5</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>Н0000095930</t>
         </is>
       </c>
     </row>
@@ -1234,20 +1292,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Рикотта шоколадно-ореховая "Красная птица", 35%, 0,2 кг, пл/с</t>
+          <t>Рикотта с шоколадом "Бонджорно", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Шоколад-орех</t>
+          <t>Шоколад</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1257,54 +1315,59 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Красная птица</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Бонджорно</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
         <v>0.2</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>6</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="n">
-        <v>350</v>
-      </c>
       <c r="L11" t="n">
+        <v>300</v>
+      </c>
+      <c r="M11" t="n">
         <v>2</v>
       </c>
-      <c r="M11" t="n">
-        <v>75</v>
-      </c>
       <c r="N11" t="n">
+        <v>36</v>
+      </c>
+      <c r="O11" t="n">
         <v>45</v>
       </c>
-      <c r="O11" t="n">
-        <v>10</v>
-      </c>
       <c r="P11" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="n">
         <v>20</v>
       </c>
-      <c r="Q11" t="n">
-        <v>15</v>
-      </c>
       <c r="R11" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S11" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T11" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U11" t="n">
-        <v>5</v>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>Н0000096629</t>
+        <v>15</v>
+      </c>
+      <c r="V11" t="n">
+        <v>5</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>Н0000095931</t>
         </is>
       </c>
     </row>
@@ -1314,16 +1377,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Рикотта "SPAR", 30%, 0,2 кг, пл/с (6 шт)</t>
+          <t>Рикотта шоколадно-ореховая "Бонджорно", 35%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
+        <v>35</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Шоколад-орех</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1333,54 +1400,59 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>SPAR</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Бонджорно</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
         <v>0.2</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>6</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="n">
-        <v>200</v>
-      </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>350</v>
       </c>
       <c r="M12" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="N12" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="O12" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="P12" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q12" t="n">
         <v>20</v>
       </c>
-      <c r="Q12" t="n">
-        <v>15</v>
-      </c>
       <c r="R12" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S12" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T12" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U12" t="n">
-        <v>5</v>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>Н0000092930</t>
+        <v>15</v>
+      </c>
+      <c r="V12" t="n">
+        <v>5</v>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>Н0000095932</t>
         </is>
       </c>
     </row>
@@ -1390,7 +1462,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Рикотта с ванилью "Бонджорно", 30%, 0,2 кг, пл/с</t>
+          <t>Рикотта с медом "Бонджорно", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1398,12 +1470,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ваниль</t>
+          <t>Мед</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1413,54 +1485,59 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>Бонджорно</t>
         </is>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0.2</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>6</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>250</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>2</v>
       </c>
-      <c r="M13" t="n">
-        <v>28</v>
-      </c>
       <c r="N13" t="n">
+        <v>50</v>
+      </c>
+      <c r="O13" t="n">
         <v>30</v>
       </c>
-      <c r="O13" t="n">
-        <v>10</v>
-      </c>
       <c r="P13" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q13" t="n">
         <v>20</v>
       </c>
-      <c r="Q13" t="n">
-        <v>15</v>
-      </c>
       <c r="R13" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T13" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U13" t="n">
-        <v>5</v>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>Н0000095930</t>
+        <v>15</v>
+      </c>
+      <c r="V13" t="n">
+        <v>5</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>Н0000097528</t>
         </is>
       </c>
     </row>
@@ -1470,20 +1547,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Рикотта с шоколадом "Бонджорно", 30%, 0,2 кг, пл/с</t>
+          <t>Рикотта "Metro Chef" 45%, 0,5 кг, пл/с</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Шоколад</t>
-        </is>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1493,54 +1566,59 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Бонджорно</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>0.2</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Metro Chef</t>
+        </is>
       </c>
       <c r="I14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J14" t="n">
         <v>6</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="n">
-        <v>300</v>
-      </c>
       <c r="L14" t="n">
-        <v>2</v>
+        <v>533</v>
       </c>
       <c r="M14" t="n">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="N14" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="O14" t="n">
         <v>10</v>
       </c>
       <c r="P14" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q14" t="n">
         <v>20</v>
       </c>
-      <c r="Q14" t="n">
-        <v>15</v>
-      </c>
       <c r="R14" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T14" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U14" t="n">
         <v>5</v>
       </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>Н0000095931</t>
+      <c r="V14" t="n">
+        <v>5</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>Н0000097279</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1628,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Рикотта шоколадно-ореховая "Бонджорно", 35%, 0,2 кг, пл/с</t>
+          <t>Рикотта шоколадно-ореховая "Aventino", 35%, 0,2 кг, п/с</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1563,7 +1641,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1573,54 +1651,59 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Бонджорно</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Aventino</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
         <v>0.2</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>6</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>350</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>2</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>75</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>45</v>
       </c>
-      <c r="O15" t="n">
-        <v>10</v>
-      </c>
       <c r="P15" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q15" t="n">
         <v>20</v>
       </c>
-      <c r="Q15" t="n">
-        <v>15</v>
-      </c>
       <c r="R15" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S15" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U15" t="n">
-        <v>5</v>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>Н0000095932</t>
+        <v>15</v>
+      </c>
+      <c r="V15" t="n">
+        <v>5</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Н0000097285</t>
         </is>
       </c>
     </row>
@@ -1630,16 +1713,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Рикотта "Глобус", 45%, 0,25 кг, пл/с</t>
+          <t>Рикотта с вишней "Бонджорно", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>45</v>
-      </c>
-      <c r="D16" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Вишня</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1649,54 +1736,59 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Глобус</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>0.25</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Бонджорно</t>
+        </is>
       </c>
       <c r="I16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J16" t="n">
         <v>6</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0</v>
       </c>
-      <c r="K16" t="n">
-        <v>400</v>
-      </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="M16" t="n">
+        <v>2</v>
+      </c>
+      <c r="N16" t="n">
         <v>50</v>
       </c>
-      <c r="N16" t="n">
-        <v>10</v>
-      </c>
       <c r="O16" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P16" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q16" t="n">
         <v>20</v>
       </c>
-      <c r="Q16" t="n">
-        <v>15</v>
-      </c>
       <c r="R16" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S16" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U16" t="n">
-        <v>5</v>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>326635016</t>
+        <v>15</v>
+      </c>
+      <c r="V16" t="n">
+        <v>5</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>Н0000098377</t>
         </is>
       </c>
     </row>
@@ -1706,20 +1798,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Рикотта с медом "Бонджорно", 30%, 0,2 кг, пл/с</t>
+          <t>Рикотта "Красная птица", 25%, 0,25 кг, пл/с</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>30</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Мед</t>
-        </is>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Да</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1729,26 +1817,28 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Бонджорно</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>0.2</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Красная птица</t>
+        </is>
       </c>
       <c r="I17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J17" t="n">
         <v>6</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="n">
-        <v>250</v>
-      </c>
       <c r="L17" t="n">
-        <v>2</v>
+        <v>300</v>
       </c>
       <c r="M17" t="n">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="N17" t="n">
         <v>30</v>
@@ -1757,26 +1847,29 @@
         <v>10</v>
       </c>
       <c r="P17" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q17" t="n">
         <v>20</v>
       </c>
-      <c r="Q17" t="n">
-        <v>15</v>
-      </c>
       <c r="R17" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T17" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U17" t="n">
         <v>5</v>
       </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>Н0000097528</t>
+      <c r="V17" t="n">
+        <v>5</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Н0000098819</t>
         </is>
       </c>
     </row>
@@ -1786,16 +1879,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Рикотта "Metro Chef" 45%, 0,5 кг, пл/с</t>
+          <t>Рикотта "SPAR", 25%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Да</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1805,54 +1898,59 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Metro Chef</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>0.5</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>SPAR</t>
+        </is>
       </c>
       <c r="I18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J18" t="n">
         <v>6</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>0</v>
       </c>
-      <c r="K18" t="n">
-        <v>400</v>
-      </c>
       <c r="L18" t="n">
+        <v>300</v>
+      </c>
+      <c r="M18" t="n">
         <v>3</v>
       </c>
-      <c r="M18" t="n">
-        <v>25</v>
-      </c>
       <c r="N18" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O18" t="n">
         <v>10</v>
       </c>
       <c r="P18" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q18" t="n">
         <v>20</v>
       </c>
-      <c r="Q18" t="n">
-        <v>15</v>
-      </c>
       <c r="R18" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U18" t="n">
         <v>5</v>
       </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>Н0000097279</t>
+      <c r="V18" t="n">
+        <v>5</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>Н0000098818</t>
         </is>
       </c>
     </row>
@@ -1862,20 +1960,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Рикотта шоколадно-ореховая "Aventino", 35%, 0,2 кг, п/с</t>
+          <t>Рикотта "ВкусВилл", 45%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Шоколад-орех</t>
-        </is>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1885,54 +1979,59 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Aventino</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ВкусВилл</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>0.2</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>6</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>0</v>
       </c>
-      <c r="K19" t="n">
-        <v>350</v>
-      </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="M19" t="n">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="N19" t="n">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="O19" t="n">
         <v>10</v>
       </c>
       <c r="P19" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q19" t="n">
         <v>20</v>
       </c>
-      <c r="Q19" t="n">
-        <v>15</v>
-      </c>
       <c r="R19" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S19" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T19" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U19" t="n">
         <v>5</v>
       </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>Н0000097285</t>
+      <c r="V19" t="n">
+        <v>5</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>Н0000098694</t>
         </is>
       </c>
     </row>
@@ -1942,20 +2041,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Рикотта с вишней "Бонджорно", 30%, 0,2 кг, пл/с</t>
+          <t>Рикотта шоколадно-ореховая "ВкусВилл", 35%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Вишня</t>
+          <t>Шоколад-орех</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1965,54 +2064,59 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Бонджорно</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ВкусВилл</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
         <v>0.2</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>6</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>0</v>
       </c>
-      <c r="K20" t="n">
-        <v>250</v>
-      </c>
       <c r="L20" t="n">
+        <v>350</v>
+      </c>
+      <c r="M20" t="n">
         <v>2</v>
       </c>
-      <c r="M20" t="n">
-        <v>50</v>
-      </c>
       <c r="N20" t="n">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="O20" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="P20" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q20" t="n">
         <v>20</v>
       </c>
-      <c r="Q20" t="n">
-        <v>15</v>
-      </c>
       <c r="R20" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S20" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T20" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U20" t="n">
-        <v>5</v>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>Н0000098377</t>
+        <v>15</v>
+      </c>
+      <c r="V20" t="n">
+        <v>5</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>Н0000098951</t>
         </is>
       </c>
     </row>
@@ -2022,16 +2126,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Рикотта "Красная птица", 25%, 0,25 кг, пл/с</t>
+          <t>Рикотта "SPAR", 30%, 0,2 кг, пл/с (6 шт)</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2041,54 +2145,59 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Красная птица</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>0.25</v>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>SPAR</t>
+        </is>
       </c>
       <c r="I21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J21" t="n">
         <v>6</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>200</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>3</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>35</v>
       </c>
-      <c r="N21" t="n">
-        <v>10</v>
-      </c>
       <c r="O21" t="n">
         <v>10</v>
       </c>
       <c r="P21" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="n">
         <v>20</v>
       </c>
-      <c r="Q21" t="n">
-        <v>15</v>
-      </c>
       <c r="R21" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T21" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U21" t="n">
         <v>5</v>
       </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>Н0000098819</t>
+      <c r="V21" t="n">
+        <v>5</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>Н0000092930</t>
         </is>
       </c>
     </row>
@@ -2098,16 +2207,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Рикотта "SPAR", 25%, 0,2 кг, пл/с</t>
+          <t>Рикотта с вишней "ВкусВилл", 30%, 0,2 кг, пл/с</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>25</v>
-      </c>
-      <c r="D22" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Вишня</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2117,54 +2230,59 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>SPAR</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ВкусВилл</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>0.2</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>6</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>0</v>
       </c>
-      <c r="K22" t="n">
-        <v>200</v>
-      </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="M22" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="N22" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="O22" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P22" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q22" t="n">
         <v>20</v>
       </c>
-      <c r="Q22" t="n">
-        <v>15</v>
-      </c>
       <c r="R22" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S22" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T22" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U22" t="n">
-        <v>5</v>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>Н0000098818</t>
+        <v>15</v>
+      </c>
+      <c r="V22" t="n">
+        <v>5</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>Н0000099328</t>
         </is>
       </c>
     </row>
@@ -2174,73 +2292,82 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Рикотта "ВкусВилл", 45%, 0,2 кг, пл/с</t>
+          <t>Рикотта с шоколадом "Unagrande", 30%, 0,18 кг, пл/с</t>
         </is>
       </c>
       <c r="C23" t="n">
+        <v>30</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Шоколад</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="J23" t="n">
+        <v>6</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>300</v>
+      </c>
+      <c r="M23" t="n">
+        <v>2</v>
+      </c>
+      <c r="N23" t="n">
+        <v>30</v>
+      </c>
+      <c r="O23" t="n">
         <v>45</v>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Рикотта</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Рикотта</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>ВкусВилл</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I23" t="n">
-        <v>6</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
-        <v>400</v>
-      </c>
-      <c r="L23" t="n">
-        <v>3</v>
-      </c>
-      <c r="M23" t="n">
-        <v>45</v>
-      </c>
-      <c r="N23" t="n">
-        <v>10</v>
-      </c>
-      <c r="O23" t="n">
-        <v>10</v>
-      </c>
       <c r="P23" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q23" t="n">
         <v>20</v>
       </c>
-      <c r="Q23" t="n">
-        <v>15</v>
-      </c>
       <c r="R23" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S23" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="T23" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U23" t="n">
-        <v>5</v>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>Н0000098694</t>
+        <v>15</v>
+      </c>
+      <c r="V23" t="n">
+        <v>5</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>Н0000086350</t>
         </is>
       </c>
     </row>
@@ -2250,20 +2377,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Рикотта шоколадно-ореховая "ВкусВилл", 35%, 0,2 кг, пл/с</t>
+          <t>Рикотта с шоколадом "Unagrande", 30%, 0,14 кг, пл/с</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Шоколад-орех</t>
+          <t>Шоколад</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Рикотта</t>
+          <t>Нет</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2273,54 +2400,549 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ВкусВилл</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="J24" t="n">
+        <v>6</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>300</v>
+      </c>
+      <c r="M24" t="n">
+        <v>2</v>
+      </c>
+      <c r="N24" t="n">
+        <v>75</v>
+      </c>
+      <c r="O24" t="n">
+        <v>45</v>
+      </c>
+      <c r="P24" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>20</v>
+      </c>
+      <c r="R24" t="n">
+        <v>15</v>
+      </c>
+      <c r="S24" t="n">
+        <v>5</v>
+      </c>
+      <c r="T24" t="n">
+        <v>10</v>
+      </c>
+      <c r="U24" t="n">
+        <v>15</v>
+      </c>
+      <c r="V24" t="n">
+        <v>5</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>Н0000094994</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Сыр мягкий Рикотта массовой долей жира в сухом веществе 25%</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>25</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Да</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Pretto</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J25" t="n">
+        <v>6</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>360</v>
+      </c>
+      <c r="M25" t="n">
+        <v>3</v>
+      </c>
+      <c r="N25" t="n">
+        <v>22</v>
+      </c>
+      <c r="O25" t="n">
+        <v>10</v>
+      </c>
+      <c r="P25" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>20</v>
+      </c>
+      <c r="R25" t="n">
+        <v>15</v>
+      </c>
+      <c r="S25" t="n">
+        <v>5</v>
+      </c>
+      <c r="T25" t="n">
+        <v>10</v>
+      </c>
+      <c r="U25" t="n">
+        <v>5</v>
+      </c>
+      <c r="V25" t="n">
+        <v>5</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>00-00006857</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Рикотта "Unagrande", 50%, 0,2 кг, пл/с</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>50</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Unagrande</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
         <v>0.2</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J26" t="n">
         <v>6</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K26" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="n">
-        <v>350</v>
-      </c>
-      <c r="L24" t="n">
+      <c r="L26" t="n">
+        <v>300</v>
+      </c>
+      <c r="M26" t="n">
         <v>2</v>
       </c>
-      <c r="M24" t="n">
-        <v>75</v>
-      </c>
-      <c r="N24" t="n">
+      <c r="N26" t="n">
+        <v>40</v>
+      </c>
+      <c r="O26" t="n">
+        <v>10</v>
+      </c>
+      <c r="P26" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>20</v>
+      </c>
+      <c r="R26" t="n">
+        <v>15</v>
+      </c>
+      <c r="S26" t="n">
+        <v>5</v>
+      </c>
+      <c r="T26" t="n">
+        <v>10</v>
+      </c>
+      <c r="U26" t="n">
+        <v>5</v>
+      </c>
+      <c r="V26" t="n">
+        <v>5</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>00-00007992</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Рикотта "Pretto", 45%, 2,5 кг, пл/в</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
         <v>45</v>
       </c>
-      <c r="O24" t="n">
-        <v>10</v>
-      </c>
-      <c r="P24" t="n">
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Pretto</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>6</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>533</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4</v>
+      </c>
+      <c r="N27" t="n">
+        <v>33</v>
+      </c>
+      <c r="O27" t="n">
+        <v>10</v>
+      </c>
+      <c r="P27" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="n">
         <v>20</v>
       </c>
-      <c r="Q24" t="n">
-        <v>15</v>
-      </c>
-      <c r="R24" t="n">
-        <v>5</v>
-      </c>
-      <c r="S24" t="n">
-        <v>10</v>
-      </c>
-      <c r="T24" t="n">
-        <v>15</v>
-      </c>
-      <c r="U24" t="n">
-        <v>5</v>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>Н0000098951</t>
+      <c r="R27" t="n">
+        <v>15</v>
+      </c>
+      <c r="S27" t="n">
+        <v>5</v>
+      </c>
+      <c r="T27" t="n">
+        <v>10</v>
+      </c>
+      <c r="U27" t="n">
+        <v>5</v>
+      </c>
+      <c r="V27" t="n">
+        <v>5</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>00-00009385</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Рикотта «МАРКЕТ», 45%, 0,2 кг, п/с</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>45</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>МАРКЕТ</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>6</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>600</v>
+      </c>
+      <c r="M28" t="n">
+        <v>4</v>
+      </c>
+      <c r="N28" t="n">
+        <v>58</v>
+      </c>
+      <c r="O28" t="n">
+        <v>10</v>
+      </c>
+      <c r="P28" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>20</v>
+      </c>
+      <c r="R28" t="n">
+        <v>15</v>
+      </c>
+      <c r="S28" t="n">
+        <v>5</v>
+      </c>
+      <c r="T28" t="n">
+        <v>10</v>
+      </c>
+      <c r="U28" t="n">
+        <v>5</v>
+      </c>
+      <c r="V28" t="n">
+        <v>5</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>00-00010060</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Рикотта с шоколадом «МАРКЕТ», 30%, 0,2 кг, п/с</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>30</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Шоколад</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>МАРКЕТ</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J29" t="n">
+        <v>6</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>300</v>
+      </c>
+      <c r="M29" t="n">
+        <v>2</v>
+      </c>
+      <c r="N29" t="n">
+        <v>36</v>
+      </c>
+      <c r="O29" t="n">
+        <v>45</v>
+      </c>
+      <c r="P29" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>20</v>
+      </c>
+      <c r="R29" t="n">
+        <v>15</v>
+      </c>
+      <c r="S29" t="n">
+        <v>5</v>
+      </c>
+      <c r="T29" t="n">
+        <v>10</v>
+      </c>
+      <c r="U29" t="n">
+        <v>15</v>
+      </c>
+      <c r="V29" t="n">
+        <v>5</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>00-00010061</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Сыр мягкий Рикотта массовой долей жира в сухом веществе 30%, 1,4 кг, в/у</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>25</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Нет</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Рикотта</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Pretto</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J30" t="n">
+        <v>6</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>360</v>
+      </c>
+      <c r="M30" t="n">
+        <v>3</v>
+      </c>
+      <c r="N30" t="n">
+        <v>22</v>
+      </c>
+      <c r="O30" t="n">
+        <v>10</v>
+      </c>
+      <c r="P30" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>20</v>
+      </c>
+      <c r="R30" t="n">
+        <v>15</v>
+      </c>
+      <c r="S30" t="n">
+        <v>5</v>
+      </c>
+      <c r="T30" t="n">
+        <v>10</v>
+      </c>
+      <c r="U30" t="n">
+        <v>5</v>
+      </c>
+      <c r="V30" t="n">
+        <v>5</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>00-00010187</t>
         </is>
       </c>
     </row>

</xml_diff>